<commit_message>
0.1.4: Adapt to kotlin open (notFinal option on blanco)
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FEFF22-AB07-2D41-A140-601B0DCAAFE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C773E3-5F0D-334E-BE08-D6EB8CE83960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="2960" windowWidth="21680" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5000" yWindow="2960" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>クラス名</t>
   </si>
@@ -216,6 +216,17 @@
   </si>
   <si>
     <t>blanco.sample.valueobjectkt.simple</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>非ファイナル</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ヒファイナル </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>○</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -300,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -373,15 +384,6 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -681,11 +683,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -701,88 +748,93 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1195,8 +1247,8 @@
   </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1207,7 +1259,8 @@
     <col min="7" max="7" width="6.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="28" style="1" customWidth="1"/>
     <col min="9" max="9" width="33.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="10" max="10" width="17.6640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
@@ -1257,7 +1310,7 @@
       <c r="C7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="11"/>
       <c r="F7" s="9"/>
     </row>
@@ -1289,12 +1342,12 @@
       <c r="G9" s="12"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:10" s="34" customFormat="1">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:10" s="33" customFormat="1">
+      <c r="A10" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="42" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="41" t="s">
         <v>27</v>
       </c>
       <c r="D10"/>
@@ -1302,12 +1355,12 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:10" s="34" customFormat="1">
-      <c r="A11" s="40" t="s">
+    <row r="11" spans="1:10" s="33" customFormat="1">
+      <c r="A11" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="42" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="41" t="s">
         <v>27</v>
       </c>
       <c r="D11"/>
@@ -1325,32 +1378,32 @@
       <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="13"/>
@@ -1373,124 +1426,129 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="15"/>
+      <c r="J16" s="52"/>
     </row>
     <row r="17" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="9"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="53" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="15"/>
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="53"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>1</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="15"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="54" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="19">
+      <c r="A20" s="18">
         <v>2</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21" t="s">
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="15"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="15"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="54"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="15"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="54"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="15"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="J17:J18"/>
     <mergeCell ref="F17:G18"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
@@ -1542,65 +1600,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="44" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="44"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="44" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="46"/>
-      <c r="D4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="45"/>
+      <c r="D4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="J5" s="48" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="50"/>
+      <c r="B6" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
0.1.5: NotFinal is changed to open, for kotlin natural behaviour.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C773E3-5F0D-334E-BE08-D6EB8CE83960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D918A1FC-860C-074C-AD05-99C781443168}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5000" yWindow="2960" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,14 +219,11 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>非ファイナル</t>
-    <rPh sb="0" eb="1">
-      <t xml:space="preserve">ヒファイナル </t>
-    </rPh>
+    <t>○</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>○</t>
+    <t>オープン</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1248,7 +1245,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1451,7 +1448,7 @@
       <c r="H17" s="15"/>
       <c r="I17" s="16"/>
       <c r="J17" s="53" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1487,7 +1484,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="28"/>
       <c r="J19" s="54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:10">

</xml_diff>

<commit_message>
3.0.15 Implement extends for kotlin specific.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
+++ b/meta/objects/BlancoValueObjectPhpSimpleSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D918A1FC-860C-074C-AD05-99C781443168}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B16507-EB76-5A48-B596-ACE714D63C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5000" yWindow="2960" windowWidth="28880" windowHeight="11800" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>クラス名</t>
   </si>
@@ -224,6 +224,29 @@
   </si>
   <si>
     <t>オープン</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(php)・継承(Kt)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>パッケージ</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>名前空間</t>
+    <rPh sb="0" eb="4">
+      <t>ナマエクウカｎ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>SealedSample</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>blanco.sample.valueobjectkt</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -308,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -725,30 +748,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -760,24 +806,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -790,15 +835,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -820,18 +863,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1242,10 +1290,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1260,7 +1308,7 @@
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19">
+    <row r="1" spans="1:8" ht="19">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1268,17 +1316,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:8">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:8">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1287,7 +1335,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1299,7 +1347,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1307,11 +1355,11 @@
       <c r="C7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="11"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1325,7 +1373,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -1339,12 +1387,12 @@
       <c r="G9" s="12"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:10" s="33" customFormat="1">
-      <c r="A10" s="39" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="38" t="s">
         <v>27</v>
       </c>
       <c r="D10"/>
@@ -1352,12 +1400,12 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:10" s="33" customFormat="1">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="38" t="s">
         <v>27</v>
       </c>
       <c r="D11"/>
@@ -1365,197 +1413,254 @@
       <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="30" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="34" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="3" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="53"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="54"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="B20"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="52"/>
-    </row>
-    <row r="17" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A17" s="51" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="46"/>
+    </row>
+    <row r="23" spans="1:15" ht="13.5" customHeight="1">
+      <c r="A23" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B23" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C23" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D23" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E23" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="50" t="s">
+      <c r="F23" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="53" t="s">
+      <c r="G23" s="50"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="53"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="18">
+    <row r="24" spans="1:15">
+      <c r="A24" s="51"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="49"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="17">
         <v>1</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C25" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20" t="s">
+      <c r="D25" s="19"/>
+      <c r="E25" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="54" t="s">
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="47" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="18">
+    <row r="26" spans="1:15">
+      <c r="A26" s="17">
         <v>2</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B26" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20" t="s">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="54"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="54"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="54"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="55"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="47"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="47"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="47"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="D23:D24"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E45" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1597,65 +1702,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="43" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="43"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="40" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="B4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="J4" s="42"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="44" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="49"/>
+      <c r="B6" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>